<commit_message>
Update IBT Liability PV Using DR.xlsx
</commit_message>
<xml_diff>
--- a/IBT Liability PV Using DR.xlsx
+++ b/IBT Liability PV Using DR.xlsx
@@ -11,6 +11,14 @@
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Present Values</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -373,7 +381,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="B1" s="1">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>